<commit_message>
add scatter chart equation
</commit_message>
<xml_diff>
--- a/lab/spreadsheets-projectile/completed-example.xlsx
+++ b/lab/spreadsheets-projectile/completed-example.xlsx
@@ -314,9 +314,6 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -334,6 +331,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1132,6 +1132,52 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$C$13:$C$27</c:f>
@@ -1401,7 +1447,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -1433,7 +1479,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -2670,8 +2716,8 @@
       <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4010026" cy="219997"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -2707,6 +2753,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -2869,7 +2916,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -3289,7 +3336,7 @@
   <dimension ref="B1:D27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3312,14 +3359,14 @@
     </row>
     <row r="2" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="6">
@@ -3330,7 +3377,7 @@
       </c>
     </row>
     <row r="5" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="2">
@@ -3341,7 +3388,7 @@
       </c>
     </row>
     <row r="6" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="3">
@@ -3352,7 +3399,7 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="2">
@@ -3363,7 +3410,7 @@
       </c>
     </row>
     <row r="8" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="3">
@@ -3377,208 +3424,208 @@
     <row r="10" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="12">
+      <c r="B13" s="11">
         <v>0</v>
       </c>
       <c r="C13" s="5">
-        <f>C$4 + C$6*COS(C$8 * PI()/180)*B13</f>
+        <f t="shared" ref="C13:C27" si="0">C$4 + C$6*COS(C$8 * PI()/180)*B13</f>
         <v>0</v>
       </c>
       <c r="D13" s="7">
-        <f>C$5+C$6*SIN(C$8*PI()/180)*B13 - 0.5*C$7 * B13*B13</f>
+        <f t="shared" ref="D13:D27" si="1">C$5+C$6*SIN(C$8*PI()/180)*B13 - 0.5*C$7 * B13*B13</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="12">
+      <c r="B14" s="11">
         <v>0.1</v>
       </c>
       <c r="C14" s="5">
-        <f>C$4 + C$6*COS(C$8 * PI()/180)*B14</f>
+        <f t="shared" si="0"/>
         <v>0.70710678118654757</v>
       </c>
       <c r="D14" s="5">
-        <f>C$5+C$6*SIN(C$8*PI()/180)*B14 - 0.5*C$7 * B14*B14</f>
+        <f t="shared" si="1"/>
         <v>0.65805678118654742</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="12">
+      <c r="B15" s="11">
         <v>0.2</v>
       </c>
       <c r="C15" s="5">
-        <f>C$4 + C$6*COS(C$8 * PI()/180)*B15</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="D15" s="5">
-        <f>C$5+C$6*SIN(C$8*PI()/180)*B15 - 0.5*C$7 * B15*B15</f>
+        <f t="shared" si="1"/>
         <v>1.2180135623730948</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="12">
+      <c r="B16" s="11">
         <v>0.3</v>
       </c>
       <c r="C16" s="5">
-        <f>C$4 + C$6*COS(C$8 * PI()/180)*B16</f>
+        <f t="shared" si="0"/>
         <v>2.1213203435596424</v>
       </c>
       <c r="D16" s="5">
-        <f>C$5+C$6*SIN(C$8*PI()/180)*B16 - 0.5*C$7 * B16*B16</f>
+        <f t="shared" si="1"/>
         <v>1.6798703435596423</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="12">
+      <c r="B17" s="11">
         <v>0.4</v>
       </c>
       <c r="C17" s="5">
-        <f>C$4 + C$6*COS(C$8 * PI()/180)*B17</f>
+        <f t="shared" si="0"/>
         <v>2.8284271247461903</v>
       </c>
       <c r="D17" s="5">
-        <f>C$5+C$6*SIN(C$8*PI()/180)*B17 - 0.5*C$7 * B17*B17</f>
+        <f t="shared" si="1"/>
         <v>2.0436271247461897</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="12">
+      <c r="B18" s="11">
         <v>0.5</v>
       </c>
       <c r="C18" s="5">
-        <f>C$4 + C$6*COS(C$8 * PI()/180)*B18</f>
+        <f t="shared" si="0"/>
         <v>3.5355339059327378</v>
       </c>
       <c r="D18" s="5">
-        <f>C$5+C$6*SIN(C$8*PI()/180)*B18 - 0.5*C$7 * B18*B18</f>
+        <f t="shared" si="1"/>
         <v>2.3092839059327375</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="12">
+      <c r="B19" s="11">
         <v>0.6</v>
       </c>
       <c r="C19" s="5">
-        <f>C$4 + C$6*COS(C$8 * PI()/180)*B19</f>
+        <f t="shared" si="0"/>
         <v>4.2426406871192848</v>
       </c>
       <c r="D19" s="5">
-        <f>C$5+C$6*SIN(C$8*PI()/180)*B19 - 0.5*C$7 * B19*B19</f>
+        <f t="shared" si="1"/>
         <v>2.4768406871192847</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="12">
+      <c r="B20" s="11">
         <v>0.7</v>
       </c>
       <c r="C20" s="5">
-        <f>C$4 + C$6*COS(C$8 * PI()/180)*B20</f>
+        <f t="shared" si="0"/>
         <v>4.9497474683058327</v>
       </c>
       <c r="D20" s="5">
-        <f>C$5+C$6*SIN(C$8*PI()/180)*B20 - 0.5*C$7 * B20*B20</f>
+        <f t="shared" si="1"/>
         <v>2.5462974683058319</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="12">
+      <c r="B21" s="11">
         <v>0.8</v>
       </c>
       <c r="C21" s="5">
-        <f>C$4 + C$6*COS(C$8 * PI()/180)*B21</f>
+        <f t="shared" si="0"/>
         <v>5.6568542494923806</v>
       </c>
       <c r="D21" s="5">
-        <f>C$5+C$6*SIN(C$8*PI()/180)*B21 - 0.5*C$7 * B21*B21</f>
+        <f t="shared" si="1"/>
         <v>2.517654249492379</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="12">
+      <c r="B22" s="11">
         <v>0.9</v>
       </c>
       <c r="C22" s="5">
-        <f>C$4 + C$6*COS(C$8 * PI()/180)*B22</f>
+        <f t="shared" si="0"/>
         <v>6.3639610306789285</v>
       </c>
       <c r="D22" s="5">
-        <f>C$5+C$6*SIN(C$8*PI()/180)*B22 - 0.5*C$7 * B22*B22</f>
+        <f t="shared" si="1"/>
         <v>2.3909110306789274</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="12">
+      <c r="B23" s="11">
         <v>1</v>
       </c>
       <c r="C23" s="5">
-        <f>C$4 + C$6*COS(C$8 * PI()/180)*B23</f>
+        <f t="shared" si="0"/>
         <v>7.0710678118654755</v>
       </c>
       <c r="D23" s="5">
-        <f>C$5+C$6*SIN(C$8*PI()/180)*B23 - 0.5*C$7 * B23*B23</f>
+        <f t="shared" si="1"/>
         <v>2.1660678118654744</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="12">
+      <c r="B24" s="11">
         <v>1.1000000000000001</v>
       </c>
       <c r="C24" s="5">
-        <f>C$4 + C$6*COS(C$8 * PI()/180)*B24</f>
+        <f t="shared" si="0"/>
         <v>7.7781745930520234</v>
       </c>
       <c r="D24" s="5">
-        <f>C$5+C$6*SIN(C$8*PI()/180)*B24 - 0.5*C$7 * B24*B24</f>
+        <f t="shared" si="1"/>
         <v>1.8431245930520213</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="12">
+      <c r="B25" s="11">
         <v>1.2</v>
       </c>
       <c r="C25" s="5">
-        <f>C$4 + C$6*COS(C$8 * PI()/180)*B25</f>
+        <f t="shared" si="0"/>
         <v>8.4852813742385695</v>
       </c>
       <c r="D25" s="5">
-        <f>C$5+C$6*SIN(C$8*PI()/180)*B25 - 0.5*C$7 * B25*B25</f>
+        <f t="shared" si="1"/>
         <v>1.4220813742385694</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="12">
+      <c r="B26" s="11">
         <v>1.3</v>
       </c>
       <c r="C26" s="5">
-        <f>C$4 + C$6*COS(C$8 * PI()/180)*B26</f>
+        <f t="shared" si="0"/>
         <v>9.1923881554251192</v>
       </c>
       <c r="D26" s="5">
-        <f>C$5+C$6*SIN(C$8*PI()/180)*B26 - 0.5*C$7 * B26*B26</f>
+        <f t="shared" si="1"/>
         <v>0.90293815542511524</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="12">
+      <c r="B27" s="11">
         <v>1.4</v>
       </c>
       <c r="C27" s="7">
-        <f>C$4 + C$6*COS(C$8 * PI()/180)*B27</f>
+        <f t="shared" si="0"/>
         <v>9.8994949366116654</v>
       </c>
       <c r="D27" s="5">
-        <f>C$5+C$6*SIN(C$8*PI()/180)*B27 - 0.5*C$7 * B27*B27</f>
+        <f t="shared" si="1"/>
         <v>0.28569493661166412</v>
       </c>
     </row>

</xml_diff>